<commit_message>
Updated Ports and constants.
</commit_message>
<xml_diff>
--- a/PortConstants.xlsx
+++ b/PortConstants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Description</t>
   </si>
@@ -51,27 +51,6 @@
     <t>Rear right Talon</t>
   </si>
   <si>
-    <t>DRIVE_LEFTSHIFTSOLIN</t>
-  </si>
-  <si>
-    <t>Left Super Shifter solenoid for pulling piston in</t>
-  </si>
-  <si>
-    <t>Left Super Shifter solenoid for pushing piston out</t>
-  </si>
-  <si>
-    <t>DRIVE_LEFTSHIFTSOLOUT</t>
-  </si>
-  <si>
-    <t>DRIVE_RIGHTSHIFTSOLIN</t>
-  </si>
-  <si>
-    <t>Right Super Shifter solenoid for pushing piston out</t>
-  </si>
-  <si>
-    <t>Right Super Shifter solenoid for pulling piston in</t>
-  </si>
-  <si>
     <t>SHOOTER_WINCHSPIKE</t>
   </si>
   <si>
@@ -153,9 +132,6 @@
     <t>Left Supershifter Encoder Pin A</t>
   </si>
   <si>
-    <t>Shooter Angle</t>
-  </si>
-  <si>
     <t>Right Supershifter Encoder Pin ?</t>
   </si>
   <si>
@@ -178,6 +154,18 @@
   </si>
   <si>
     <t>Winch Solenoid Out</t>
+  </si>
+  <si>
+    <t>DRIVE_SUPERSHIFTSOLIN</t>
+  </si>
+  <si>
+    <t>DRIVE_SUPERSHIFTSOLOUT</t>
+  </si>
+  <si>
+    <t>Super Shifter solenoid for pulling piston in</t>
+  </si>
+  <si>
+    <t>Super Shifter solenoid for pushing piston out</t>
   </si>
 </sst>
 </file>
@@ -514,11 +502,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -532,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -543,132 +529,132 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -676,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -690,7 +676,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -704,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -718,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -729,181 +715,142 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D29">
-    <sortCondition ref="B2:B29"/>
-    <sortCondition ref="C2:C29"/>
+  <sortState ref="A2:D27">
+    <sortCondition ref="B2:B27"/>
+    <sortCondition ref="C2:C27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>